<commit_message>
data driven testing excel
</commit_message>
<xml_diff>
--- a/src/test/resources/testdatas.xlsx
+++ b/src/test/resources/testdatas.xlsx
@@ -11,15 +11,88 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>Python code</t>
   </si>
   <si>
-    <t>print ("Hello")</t>
-  </si>
-  <si>
-    <t>print ("Welcome")</t>
+    <t>Invalid Python code</t>
+  </si>
+  <si>
+    <t>def search(input_list, num):
+    if num in input_list:
+        return "Element Found"
+    else:
+        return "Not Found"
+input_list = [12, 23, 45, 67, 6, 90]
+num = 6
+print(search(input_list, num))</t>
+  </si>
+  <si>
+    <t>print Hello</t>
+  </si>
+  <si>
+    <t>def find_max_consecutive_ones(nums):
+    max_count = 0
+    current_count = 0
+    for num in nums:
+        if num == 1:
+            current_count += 1
+        else:
+            if current_count &gt; max_count:
+                max_count = current_count
+            current_count = 0
+    # Final check in case the longest sequence ends at the end of the array
+    if current_count &gt; max_count:
+        max_count = current_count
+    return max_count
+# Example usage
+nums = [1, 1, 0, 1, 1, 1]
+print("Maximum consecutive 1's:", find_max_consecutive_ones(nums))</t>
+  </si>
+  <si>
+    <t>def count_numbers_with_even_digits(nums):
+    def count_digits(n):
+        return len(str(n))
+    even_digit_count = 0
+    for num in nums:
+        if count_digits(num) % 2 == 0:
+            even_digit_count += 1
+    return even_digit_count
+# Example usage
+nums = [12, 345, 2, 6, 7896]
+print("Count of numbers with even digits:", count_numbers_with_even_digits(nums))</t>
+  </si>
+  <si>
+    <t>print Welcome seleniumsquad</t>
+  </si>
+  <si>
+    <t>def sorted_squares(nums):
+    # Initialize pointers and result array
+    left, right = 0, len(nums) - 1
+    result = [0] * len(nums)
+    # Position to insert the squared values, starting from the end of the result array
+    position = len(nums) - 1
+    while left &lt;= right:
+        # Square the values at the left and right pointers
+        left_square = nums[left] ** 2
+        right_square = nums[right] ** 2
+        # Place the larger square at the current position
+        if left_square &gt; right_square:
+            result[position] = left_square
+            left += 1
+        else:
+            result[position] = right_square
+            right -= 1
+        # Move the position pointer to the left
+        position -= 1
+    return result
+# Example usage
+nums = [-4, -1, 0, 3, 10]
+print("Sorted squares:", sorted_squares(nums))</t>
+  </si>
+  <si>
+    <t>print numpyninja</t>
   </si>
 </sst>
 </file>
@@ -276,22 +349,48 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="13.88"/>
+    <col customWidth="1" min="1" max="1" width="55.5"/>
+    <col customWidth="1" min="2" max="2" width="23.25"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>